<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - add_percentage_growth_by_sector_row change
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df_fixed_1.xlsx
+++ b/create_forecast_basic/utils/monitoring_df_fixed_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="1397">
   <si>
     <t>2020</t>
   </si>
@@ -5301,14 +5301,14 @@
       <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
+      <c r="C46" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1388</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -6729,11 +6729,11 @@
       <c r="A148" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C148" t="s">
-        <v>1388</v>
-      </c>
-      <c r="D148" t="s">
-        <v>1388</v>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148">
+        <v>0</v>
       </c>
       <c r="E148">
         <v>129.4654903995849</v>
@@ -8619,14 +8619,14 @@
       <c r="A283" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="C283" t="s">
-        <v>1388</v>
-      </c>
-      <c r="D283" t="s">
-        <v>1388</v>
-      </c>
-      <c r="E283" t="s">
-        <v>1388</v>
+      <c r="C283">
+        <v>0</v>
+      </c>
+      <c r="D283">
+        <v>0</v>
+      </c>
+      <c r="E283">
+        <v>0</v>
       </c>
     </row>
     <row r="284" spans="1:5">
@@ -8706,11 +8706,11 @@
       <c r="C289">
         <v>0.8743169398907104</v>
       </c>
-      <c r="D289" t="s">
-        <v>1388</v>
-      </c>
-      <c r="E289" t="s">
-        <v>1388</v>
+      <c r="D289">
+        <v>0</v>
+      </c>
+      <c r="E289">
+        <v>0</v>
       </c>
     </row>
     <row r="290" spans="1:5">
@@ -8748,11 +8748,11 @@
       <c r="C292">
         <v>0.8686210640608035</v>
       </c>
-      <c r="D292" t="s">
-        <v>1388</v>
-      </c>
-      <c r="E292" t="s">
-        <v>1388</v>
+      <c r="D292">
+        <v>0</v>
+      </c>
+      <c r="E292">
+        <v>0</v>
       </c>
     </row>
     <row r="293" spans="1:5">
@@ -8835,8 +8835,8 @@
       <c r="D298">
         <v>1.326086956521744</v>
       </c>
-      <c r="E298" t="s">
-        <v>1388</v>
+      <c r="E298">
+        <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:5">

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - cleanup
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df_fixed_1.xlsx
+++ b/create_forecast_basic/utils/monitoring_df_fixed_1.xlsx
@@ -100,22 +100,22 @@
     <t>taz_num_count</t>
   </si>
   <si>
-    <t>percentage growth pop 2020-2025</t>
-  </si>
-  <si>
-    <t>percentage growth pop 2025-2030</t>
-  </si>
-  <si>
-    <t>percentage growth pop 2030-2035</t>
-  </si>
-  <si>
-    <t>percentage growth pop 2035-2040</t>
-  </si>
-  <si>
-    <t>percentage growth pop 2040-2045</t>
-  </si>
-  <si>
-    <t>percentage growth pop 2045-2050</t>
+    <t>percentage growth pop_without_dorms_yeshiva 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth pop_without_dorms_yeshiva 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth pop_without_dorms_yeshiva 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth pop_without_dorms_yeshiva 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth pop_without_dorms_yeshiva 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth pop_without_dorms_yeshiva 2045-2050</t>
   </si>
   <si>
     <t>percentage growth univ 2020-2025</t>

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - add_pop_division_emp_okev_by_SCHN_NAME
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df_fixed_1.xlsx
+++ b/create_forecast_basic/utils/monitoring_df_fixed_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="1509">
   <si>
     <t>2020</t>
   </si>
@@ -4193,6 +4193,342 @@
   </si>
   <si>
     <t>total_emp at שומרון in 2050</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at 0 in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at 0 in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at א-טור in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at א-טור in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at אבו טור סילוא in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at אבו טור סילוא in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at אזור תעשיה גב in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at אזור תעשיה גב in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at אזור תעשיה עט in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at אזור תעשיה עט in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at בית הכרם in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at בית הכרם in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at בית צפפא,שרפת in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at בית צפפא,שרפת in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at בקעה מושבות in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at בקעה מושבות in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at גבעת המטוס in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at גבעת המטוס in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at גבעת משואה in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at גבעת משואה in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at גילה in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at גילה in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at הגבעה הצרפתי in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at הגבעה הצרפתי in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at העיר העתיקה in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at העיר העתיקה in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at הקריות של ירו in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at הקריות של ירו in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at הר החוצבים in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at הר החוצבים in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at הר הצופים in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at הר הצופים in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at הר נוף in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at הר נוף in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at חומת שמואל - ה in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at חומת שמואל - ה in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at חומת שמואל-מע in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at חומת שמואל-מע in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at טלביה רחביה in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at טלביה רחביה in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at יובלים גנים in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at יובלים גנים in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at כניסה לעיר in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at כניסה לעיר in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at כניסה לעיר - ק in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at כניסה לעיר - ק in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at כפר עקב in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at כפר עקב in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מורשה in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מורשה in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מחנה שועפט in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מחנה שועפט in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מנחת - מלחה in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מנחת - מלחה in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מעלות דפנה in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מעלות דפנה in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מער in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מער in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מער חרדי in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מער חרדי in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מער מזרח ואדי in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מער מזרח ואדי in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מקור ברוך in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מקור ברוך in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מרכז רפואי הד in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at מרכז רפואי הד in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at נוה יעקב in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at נוה יעקב in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at נחלאות שערי ח in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at נחלאות שערי ח in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at ניות -גבעת מר in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at ניות -גבעת מר in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at סנהדריה רמת א in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at סנהדריה רמת א in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at עין כרם in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at עין כרם in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at עיסאוויה in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at עיסאוויה in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at פסגת זאב in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at פסגת זאב in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at פת - קטמונים in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at פת - קטמונים in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at צור באהר מורח in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at צור באהר מורח in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at קטמון הישנה in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at קטמון הישנה in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at קריית הממשלה- in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at קריית הממשלה- in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at קריית משה -גב in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at קריית משה -גב in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at ראס אל עמד - ג' in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at ראס אל עמד - ג' in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at רכס לבן in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at רכס לבן in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at רמות in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at רמות in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at רמת שלמה in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at רמת שלמה in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at רמת שרת - בית in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at רמת שרת - בית in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at רסקו in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at רסקו in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at שדה התעופה עט in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at שדה התעופה עט in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at שועפאט - בית in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at שועפאט - בית in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at תלפיות in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at תלפיות in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at תלפיות ארנונ in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at תלפיות ארנונ in 2025</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at תלפיות מזרח in 2020</t>
+  </si>
+  <si>
+    <t>pop division emp_okev at תלפיות מזרח in 2025</t>
   </si>
   <si>
     <t>1,758,461</t>
@@ -4604,7 +4940,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1376"/>
+  <dimension ref="A1:E1488"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4629,16 +4965,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1379</v>
+        <v>1491</v>
       </c>
       <c r="C2" t="s">
-        <v>1379</v>
+        <v>1491</v>
       </c>
       <c r="D2" t="s">
-        <v>1379</v>
+        <v>1491</v>
       </c>
       <c r="E2" t="s">
-        <v>1379</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4646,13 +4982,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>1384</v>
+        <v>1496</v>
       </c>
       <c r="D3" t="s">
-        <v>1389</v>
+        <v>1501</v>
       </c>
       <c r="E3" t="s">
-        <v>1393</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4660,16 +4996,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>1380</v>
+        <v>1492</v>
       </c>
       <c r="C4" t="s">
-        <v>1380</v>
+        <v>1492</v>
       </c>
       <c r="D4" t="s">
-        <v>1380</v>
+        <v>1492</v>
       </c>
       <c r="E4" t="s">
-        <v>1380</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4677,13 +5013,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>1385</v>
+        <v>1497</v>
       </c>
       <c r="D5" t="s">
-        <v>1390</v>
+        <v>1502</v>
       </c>
       <c r="E5" t="s">
-        <v>1394</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4776,16 +5112,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>1381</v>
+        <v>1493</v>
       </c>
       <c r="C11" t="s">
-        <v>1381</v>
+        <v>1493</v>
       </c>
       <c r="D11" t="s">
-        <v>1381</v>
+        <v>1493</v>
       </c>
       <c r="E11" t="s">
-        <v>1381</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -4793,13 +5129,13 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>1381</v>
+        <v>1493</v>
       </c>
       <c r="D12" t="s">
-        <v>1381</v>
+        <v>1493</v>
       </c>
       <c r="E12" t="s">
-        <v>1381</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -4807,16 +5143,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>1382</v>
+        <v>1494</v>
       </c>
       <c r="C13" t="s">
-        <v>1382</v>
+        <v>1494</v>
       </c>
       <c r="D13" t="s">
-        <v>1382</v>
+        <v>1494</v>
       </c>
       <c r="E13" t="s">
-        <v>1382</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -4824,13 +5160,13 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>1386</v>
+        <v>1498</v>
       </c>
       <c r="D14" t="s">
-        <v>1391</v>
+        <v>1503</v>
       </c>
       <c r="E14" t="s">
-        <v>1395</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -4838,16 +5174,16 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>1383</v>
+        <v>1495</v>
       </c>
       <c r="C15" t="s">
-        <v>1383</v>
+        <v>1495</v>
       </c>
       <c r="D15" t="s">
-        <v>1383</v>
+        <v>1495</v>
       </c>
       <c r="E15" t="s">
-        <v>1383</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -4855,13 +5191,13 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>1387</v>
+        <v>1499</v>
       </c>
       <c r="D16" t="s">
-        <v>1392</v>
+        <v>1504</v>
       </c>
       <c r="E16" t="s">
-        <v>1396</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5302,13 +5638,13 @@
         <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>1388</v>
+        <v>1500</v>
       </c>
       <c r="D46" t="s">
-        <v>1388</v>
+        <v>1500</v>
       </c>
       <c r="E46" t="s">
-        <v>1388</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -23929,6 +24265,1574 @@
       </c>
       <c r="E1376">
         <v>9117.43646116608</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:5">
+      <c r="A1377" s="1" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C1377">
+        <v>10.61797177433101</v>
+      </c>
+      <c r="D1377">
+        <v>10.61797177433101</v>
+      </c>
+      <c r="E1377">
+        <v>10.61797177433101</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:5">
+      <c r="A1378" s="1" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C1378">
+        <v>48.66136791876972</v>
+      </c>
+      <c r="D1378">
+        <v>50.26030791605782</v>
+      </c>
+      <c r="E1378">
+        <v>49.7684289776571</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:5">
+      <c r="A1379" s="1" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C1379">
+        <v>8.879335743536435</v>
+      </c>
+      <c r="D1379">
+        <v>8.879335743536435</v>
+      </c>
+      <c r="E1379">
+        <v>8.879335743536435</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:5">
+      <c r="A1380" s="1" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C1380">
+        <v>8.97809595681324</v>
+      </c>
+      <c r="D1380">
+        <v>8.97809595681324</v>
+      </c>
+      <c r="E1380">
+        <v>8.978095956813242</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:5">
+      <c r="A1381" s="1" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C1381">
+        <v>10.48817622266559</v>
+      </c>
+      <c r="D1381">
+        <v>10.48817622266559</v>
+      </c>
+      <c r="E1381">
+        <v>10.48817622266559</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:5">
+      <c r="A1382" s="1" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C1382">
+        <v>10.64197920075806</v>
+      </c>
+      <c r="D1382">
+        <v>10.65733287027282</v>
+      </c>
+      <c r="E1382">
+        <v>10.65123788087779</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:5">
+      <c r="A1383" s="1" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C1383">
+        <v>0</v>
+      </c>
+      <c r="D1383">
+        <v>0</v>
+      </c>
+      <c r="E1383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:5">
+      <c r="A1384" s="1" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C1384">
+        <v>0</v>
+      </c>
+      <c r="D1384">
+        <v>0</v>
+      </c>
+      <c r="E1384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:5">
+      <c r="A1385" s="1" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C1385">
+        <v>0</v>
+      </c>
+      <c r="D1385">
+        <v>0</v>
+      </c>
+      <c r="E1385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:5">
+      <c r="A1386" s="1" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C1386">
+        <v>0</v>
+      </c>
+      <c r="D1386">
+        <v>0</v>
+      </c>
+      <c r="E1386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:5">
+      <c r="A1387" s="1" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C1387">
+        <v>7.124781198522624</v>
+      </c>
+      <c r="D1387">
+        <v>7.124781198522624</v>
+      </c>
+      <c r="E1387">
+        <v>7.124781198522624</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:5">
+      <c r="A1388" s="1" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C1388">
+        <v>7.308352879444294</v>
+      </c>
+      <c r="D1388">
+        <v>6.891837625228979</v>
+      </c>
+      <c r="E1388">
+        <v>6.961116780234643</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:5">
+      <c r="A1389" s="1" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C1389">
+        <v>11.71001852449868</v>
+      </c>
+      <c r="D1389">
+        <v>11.71001852449868</v>
+      </c>
+      <c r="E1389">
+        <v>11.71001852449868</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:5">
+      <c r="A1390" s="1" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C1390">
+        <v>11.90347984974643</v>
+      </c>
+      <c r="D1390">
+        <v>11.90347984974643</v>
+      </c>
+      <c r="E1390">
+        <v>11.90347984974643</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:5">
+      <c r="A1391" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C1391">
+        <v>22.00711043041655</v>
+      </c>
+      <c r="D1391">
+        <v>22.00711043041655</v>
+      </c>
+      <c r="E1391">
+        <v>22.00711043041655</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:5">
+      <c r="A1392" s="1" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C1392">
+        <v>22.15309767411908</v>
+      </c>
+      <c r="D1392">
+        <v>22.95406507450567</v>
+      </c>
+      <c r="E1392">
+        <v>22.69873846913899</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:5">
+      <c r="A1393" s="1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C1393">
+        <v>0</v>
+      </c>
+      <c r="D1393">
+        <v>0</v>
+      </c>
+      <c r="E1393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:5">
+      <c r="A1394" s="1" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C1394">
+        <v>0</v>
+      </c>
+      <c r="D1394">
+        <v>0</v>
+      </c>
+      <c r="E1394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:5">
+      <c r="A1395" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C1395">
+        <v>5.585780140371284</v>
+      </c>
+      <c r="D1395">
+        <v>5.585780140371284</v>
+      </c>
+      <c r="E1395">
+        <v>5.585780140371284</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:5">
+      <c r="A1396" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C1396">
+        <v>6.280991735537189</v>
+      </c>
+      <c r="D1396">
+        <v>6.28099173553719</v>
+      </c>
+      <c r="E1396">
+        <v>6.28099173553719</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:5">
+      <c r="A1397" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C1397">
+        <v>5.351811824539101</v>
+      </c>
+      <c r="D1397">
+        <v>5.351811824539101</v>
+      </c>
+      <c r="E1397">
+        <v>5.351811824539101</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:5">
+      <c r="A1398" s="1" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C1398">
+        <v>5.728047129564301</v>
+      </c>
+      <c r="D1398">
+        <v>5.72773368218265</v>
+      </c>
+      <c r="E1398">
+        <v>5.727903274549295</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:5">
+      <c r="A1399" s="1" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C1399">
+        <v>39.23725427102401</v>
+      </c>
+      <c r="D1399">
+        <v>39.23725427102401</v>
+      </c>
+      <c r="E1399">
+        <v>39.23725427102401</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:5">
+      <c r="A1400" s="1" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C1400">
+        <v>40.49165572956781</v>
+      </c>
+      <c r="D1400">
+        <v>40.94104047252055</v>
+      </c>
+      <c r="E1400">
+        <v>40.93406273939863</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:5">
+      <c r="A1401" s="1" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C1401">
+        <v>0</v>
+      </c>
+      <c r="D1401">
+        <v>0</v>
+      </c>
+      <c r="E1401">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:5">
+      <c r="A1402" s="1" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C1402">
+        <v>0</v>
+      </c>
+      <c r="D1402">
+        <v>0</v>
+      </c>
+      <c r="E1402">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:5">
+      <c r="A1403" s="1" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C1403">
+        <v>20.70118699601915</v>
+      </c>
+      <c r="D1403">
+        <v>20.70118699601915</v>
+      </c>
+      <c r="E1403">
+        <v>20.70118699601915</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:5">
+      <c r="A1404" s="1" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C1404">
+        <v>24.91431893195359</v>
+      </c>
+      <c r="D1404">
+        <v>24.91280982354486</v>
+      </c>
+      <c r="E1404">
+        <v>24.91152165368718</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:5">
+      <c r="A1405" s="1" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C1405">
+        <v>0</v>
+      </c>
+      <c r="D1405">
+        <v>0</v>
+      </c>
+      <c r="E1405">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:5">
+      <c r="A1406" s="1" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C1406">
+        <v>0</v>
+      </c>
+      <c r="D1406">
+        <v>0</v>
+      </c>
+      <c r="E1406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:5">
+      <c r="A1407" s="1" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C1407">
+        <v>0</v>
+      </c>
+      <c r="D1407">
+        <v>0</v>
+      </c>
+      <c r="E1407">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:5">
+      <c r="A1408" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C1408">
+        <v>0</v>
+      </c>
+      <c r="D1408">
+        <v>0</v>
+      </c>
+      <c r="E1408">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:5">
+      <c r="A1409" s="1" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C1409">
+        <v>14.66547261650109</v>
+      </c>
+      <c r="D1409">
+        <v>14.66547261650109</v>
+      </c>
+      <c r="E1409">
+        <v>14.66547261650109</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:5">
+      <c r="A1410" s="1" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C1410">
+        <v>15.1941214789956</v>
+      </c>
+      <c r="D1410">
+        <v>15.1941214789956</v>
+      </c>
+      <c r="E1410">
+        <v>15.1941214789956</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:5">
+      <c r="A1411" s="1" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C1411">
+        <v>6.944442962067281</v>
+      </c>
+      <c r="D1411">
+        <v>6.944442962067281</v>
+      </c>
+      <c r="E1411">
+        <v>6.944442962067281</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:5">
+      <c r="A1412" s="1" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C1412">
+        <v>6.942148760330578</v>
+      </c>
+      <c r="D1412">
+        <v>6.942148760330582</v>
+      </c>
+      <c r="E1412">
+        <v>6.942148760330578</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:5">
+      <c r="A1413" s="1" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C1413">
+        <v>0</v>
+      </c>
+      <c r="D1413">
+        <v>0</v>
+      </c>
+      <c r="E1413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:5">
+      <c r="A1414" s="1" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C1414">
+        <v>0</v>
+      </c>
+      <c r="D1414">
+        <v>0</v>
+      </c>
+      <c r="E1414">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:5">
+      <c r="A1415" s="1" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C1415">
+        <v>7.347476667204568</v>
+      </c>
+      <c r="D1415">
+        <v>7.347476667204568</v>
+      </c>
+      <c r="E1415">
+        <v>7.347476667204568</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:5">
+      <c r="A1416" s="1" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C1416">
+        <v>6.738142506191168</v>
+      </c>
+      <c r="D1416">
+        <v>6.717886164423779</v>
+      </c>
+      <c r="E1416">
+        <v>6.718213713655519</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:5">
+      <c r="A1417" s="1" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C1417">
+        <v>5.202732404265584</v>
+      </c>
+      <c r="D1417">
+        <v>5.202732404265584</v>
+      </c>
+      <c r="E1417">
+        <v>5.202732404265584</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:5">
+      <c r="A1418" s="1" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C1418">
+        <v>5.692485246231844</v>
+      </c>
+      <c r="D1418">
+        <v>5.689438851389011</v>
+      </c>
+      <c r="E1418">
+        <v>5.68618828405399</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:5">
+      <c r="A1419" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C1419">
+        <v>0</v>
+      </c>
+      <c r="D1419">
+        <v>0</v>
+      </c>
+      <c r="E1419">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:5">
+      <c r="A1420" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C1420">
+        <v>0</v>
+      </c>
+      <c r="D1420">
+        <v>0</v>
+      </c>
+      <c r="E1420">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:5">
+      <c r="A1421" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C1421">
+        <v>91.24879455885682</v>
+      </c>
+      <c r="D1421">
+        <v>91.24879455885682</v>
+      </c>
+      <c r="E1421">
+        <v>91.24879455885682</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:5">
+      <c r="A1422" s="1" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C1422">
+        <v>90.56489963902756</v>
+      </c>
+      <c r="D1422">
+        <v>91.28950915822267</v>
+      </c>
+      <c r="E1422">
+        <v>91.39560998488896</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:5">
+      <c r="A1423" s="1" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C1423">
+        <v>12.08791208791209</v>
+      </c>
+      <c r="D1423">
+        <v>12.08791208791209</v>
+      </c>
+      <c r="E1423">
+        <v>12.08791208791209</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:5">
+      <c r="A1424" s="1" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C1424">
+        <v>11.78516286509618</v>
+      </c>
+      <c r="D1424">
+        <v>11.78516286509618</v>
+      </c>
+      <c r="E1424">
+        <v>11.78516286509618</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:5">
+      <c r="A1425" s="1" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C1425">
+        <v>0</v>
+      </c>
+      <c r="D1425">
+        <v>0</v>
+      </c>
+      <c r="E1425">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:5">
+      <c r="A1426" s="1" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C1426">
+        <v>0</v>
+      </c>
+      <c r="D1426">
+        <v>0</v>
+      </c>
+      <c r="E1426">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:5">
+      <c r="A1427" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C1427">
+        <v>11.74716806238538</v>
+      </c>
+      <c r="D1427">
+        <v>11.74716806238538</v>
+      </c>
+      <c r="E1427">
+        <v>11.74716806238538</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:5">
+      <c r="A1428" s="1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C1428">
+        <v>11.44824005909651</v>
+      </c>
+      <c r="D1428">
+        <v>11.44704172880582</v>
+      </c>
+      <c r="E1428">
+        <v>11.44705978651874</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:5">
+      <c r="A1429" s="1" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C1429">
+        <v>6.832876037424109</v>
+      </c>
+      <c r="D1429">
+        <v>6.832876037424109</v>
+      </c>
+      <c r="E1429">
+        <v>6.832876037424109</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:5">
+      <c r="A1430" s="1" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C1430">
+        <v>7.767185784048269</v>
+      </c>
+      <c r="D1430">
+        <v>7.767185784048263</v>
+      </c>
+      <c r="E1430">
+        <v>7.767185784048269</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:5">
+      <c r="A1431" s="1" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C1431">
+        <v>18.77653961963095</v>
+      </c>
+      <c r="D1431">
+        <v>18.77653961963095</v>
+      </c>
+      <c r="E1431">
+        <v>18.77653961963095</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:5">
+      <c r="A1432" s="1" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C1432">
+        <v>19.44024615580287</v>
+      </c>
+      <c r="D1432">
+        <v>19.31312751089166</v>
+      </c>
+      <c r="E1432">
+        <v>19.32225336826691</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:5">
+      <c r="A1433" s="1" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C1433">
+        <v>0</v>
+      </c>
+      <c r="D1433">
+        <v>0</v>
+      </c>
+      <c r="E1433">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:5">
+      <c r="A1434" s="1" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C1434">
+        <v>0</v>
+      </c>
+      <c r="D1434">
+        <v>0</v>
+      </c>
+      <c r="E1434">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:5">
+      <c r="A1435" s="1" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C1435">
+        <v>32.70664157449798</v>
+      </c>
+      <c r="D1435">
+        <v>32.70664157449798</v>
+      </c>
+      <c r="E1435">
+        <v>32.70664157449798</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:5">
+      <c r="A1436" s="1" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C1436">
+        <v>35.5682969497193</v>
+      </c>
+      <c r="D1436">
+        <v>35.34646507018998</v>
+      </c>
+      <c r="E1436">
+        <v>35.39803257083106</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:5">
+      <c r="A1437" s="1" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C1437">
+        <v>0</v>
+      </c>
+      <c r="D1437">
+        <v>0</v>
+      </c>
+      <c r="E1437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:5">
+      <c r="A1438" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="C1438">
+        <v>0</v>
+      </c>
+      <c r="D1438">
+        <v>0</v>
+      </c>
+      <c r="E1438">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:5">
+      <c r="A1439" s="1" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C1439">
+        <v>0</v>
+      </c>
+      <c r="D1439">
+        <v>0</v>
+      </c>
+      <c r="E1439">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:5">
+      <c r="A1440" s="1" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C1440">
+        <v>0</v>
+      </c>
+      <c r="D1440">
+        <v>0</v>
+      </c>
+      <c r="E1440">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:5">
+      <c r="A1441" s="1" t="s">
+        <v>1443</v>
+      </c>
+      <c r="C1441">
+        <v>0</v>
+      </c>
+      <c r="D1441">
+        <v>0</v>
+      </c>
+      <c r="E1441">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:5">
+      <c r="A1442" s="1" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C1442">
+        <v>0</v>
+      </c>
+      <c r="D1442">
+        <v>0</v>
+      </c>
+      <c r="E1442">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:5">
+      <c r="A1443" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C1443">
+        <v>16.39725505146778</v>
+      </c>
+      <c r="D1443">
+        <v>16.39725505146778</v>
+      </c>
+      <c r="E1443">
+        <v>16.39725505146778</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:5">
+      <c r="A1444" s="1" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C1444">
+        <v>18.45514042445038</v>
+      </c>
+      <c r="D1444">
+        <v>18.49033157702685</v>
+      </c>
+      <c r="E1444">
+        <v>18.48548096986664</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:5">
+      <c r="A1445" s="1" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C1445">
+        <v>102.0295600503881</v>
+      </c>
+      <c r="D1445">
+        <v>102.0295600503881</v>
+      </c>
+      <c r="E1445">
+        <v>102.0295600503881</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:5">
+      <c r="A1446" s="1" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C1446">
+        <v>113.8681090059341</v>
+      </c>
+      <c r="D1446">
+        <v>115.1956358320139</v>
+      </c>
+      <c r="E1446">
+        <v>118.8240836730507</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:5">
+      <c r="A1447" s="1" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C1447">
+        <v>5.945316652078143</v>
+      </c>
+      <c r="D1447">
+        <v>5.945316652078143</v>
+      </c>
+      <c r="E1447">
+        <v>5.945316652078143</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:5">
+      <c r="A1448" s="1" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C1448">
+        <v>6.942148760330579</v>
+      </c>
+      <c r="D1448">
+        <v>6.942148760330581</v>
+      </c>
+      <c r="E1448">
+        <v>6.942148760330581</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:5">
+      <c r="A1449" s="1" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C1449">
+        <v>13.74233004967821</v>
+      </c>
+      <c r="D1449">
+        <v>13.74233004967821</v>
+      </c>
+      <c r="E1449">
+        <v>13.74233004967821</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:5">
+      <c r="A1450" s="1" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C1450">
+        <v>16.76729304575607</v>
+      </c>
+      <c r="D1450">
+        <v>16.670043633783</v>
+      </c>
+      <c r="E1450">
+        <v>16.49860679659169</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:5">
+      <c r="A1451" s="1" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C1451">
+        <v>4.505540946656641</v>
+      </c>
+      <c r="D1451">
+        <v>4.505540946656641</v>
+      </c>
+      <c r="E1451">
+        <v>4.505540946656641</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:5">
+      <c r="A1452" s="1" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C1452">
+        <v>4.753474830954171</v>
+      </c>
+      <c r="D1452">
+        <v>4.75347483095417</v>
+      </c>
+      <c r="E1452">
+        <v>4.753474830954172</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:5">
+      <c r="A1453" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C1453">
+        <v>10.99870325494772</v>
+      </c>
+      <c r="D1453">
+        <v>10.99870325494772</v>
+      </c>
+      <c r="E1453">
+        <v>10.99870325494772</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:5">
+      <c r="A1454" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C1454">
+        <v>11.16113328814083</v>
+      </c>
+      <c r="D1454">
+        <v>11.16113328814083</v>
+      </c>
+      <c r="E1454">
+        <v>11.16113328814084</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:5">
+      <c r="A1455" s="1" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C1455">
+        <v>7.457743220880475</v>
+      </c>
+      <c r="D1455">
+        <v>7.457743220880475</v>
+      </c>
+      <c r="E1455">
+        <v>7.457743220880475</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:5">
+      <c r="A1456" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C1456">
+        <v>7.623295056673723</v>
+      </c>
+      <c r="D1456">
+        <v>7.64009813006245</v>
+      </c>
+      <c r="E1456">
+        <v>7.636071415732046</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:5">
+      <c r="A1457" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C1457">
+        <v>5.811428131537058</v>
+      </c>
+      <c r="D1457">
+        <v>5.811428131537058</v>
+      </c>
+      <c r="E1457">
+        <v>5.811428131537058</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:5">
+      <c r="A1458" s="1" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C1458">
+        <v>6.172487281127843</v>
+      </c>
+      <c r="D1458">
+        <v>6.099233051633656</v>
+      </c>
+      <c r="E1458">
+        <v>6.119577814703307</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:5">
+      <c r="A1459" s="1" t="s">
+        <v>1461</v>
+      </c>
+      <c r="C1459">
+        <v>9.504076162580008</v>
+      </c>
+      <c r="D1459">
+        <v>9.504076162580008</v>
+      </c>
+      <c r="E1459">
+        <v>9.504076162580008</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:5">
+      <c r="A1460" s="1" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C1460">
+        <v>9.552561591347882</v>
+      </c>
+      <c r="D1460">
+        <v>9.552347929157344</v>
+      </c>
+      <c r="E1460">
+        <v>9.552350672556532</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:5">
+      <c r="A1461" s="1" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C1461">
+        <v>3.956323603879162</v>
+      </c>
+      <c r="D1461">
+        <v>3.956323603879162</v>
+      </c>
+      <c r="E1461">
+        <v>3.956323603879162</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:5">
+      <c r="A1462" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C1462">
+        <v>4.171014397564975</v>
+      </c>
+      <c r="D1462">
+        <v>4.172972218938142</v>
+      </c>
+      <c r="E1462">
+        <v>4.172428755729251</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:5">
+      <c r="A1463" s="1" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C1463">
+        <v>0</v>
+      </c>
+      <c r="D1463">
+        <v>0</v>
+      </c>
+      <c r="E1463">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:5">
+      <c r="A1464" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C1464">
+        <v>0</v>
+      </c>
+      <c r="D1464">
+        <v>0</v>
+      </c>
+      <c r="E1464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:5">
+      <c r="A1465" s="1" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C1465">
+        <v>221.3329223895845</v>
+      </c>
+      <c r="D1465">
+        <v>221.3329223895845</v>
+      </c>
+      <c r="E1465">
+        <v>221.3329223895845</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:5">
+      <c r="A1466" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C1466">
+        <v>237.4078039230274</v>
+      </c>
+      <c r="D1466">
+        <v>230.1613518100752</v>
+      </c>
+      <c r="E1466">
+        <v>234.523447818702</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:5">
+      <c r="A1467" s="1" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C1467">
+        <v>10.47478667238044</v>
+      </c>
+      <c r="D1467">
+        <v>10.47478667238044</v>
+      </c>
+      <c r="E1467">
+        <v>10.47478667238044</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:5">
+      <c r="A1468" s="1" t="s">
+        <v>1470</v>
+      </c>
+      <c r="C1468">
+        <v>10.38830448361933</v>
+      </c>
+      <c r="D1468">
+        <v>10.38663976374064</v>
+      </c>
+      <c r="E1468">
+        <v>10.38646121365346</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:5">
+      <c r="A1469" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C1469">
+        <v>0</v>
+      </c>
+      <c r="D1469">
+        <v>0</v>
+      </c>
+      <c r="E1469">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:5">
+      <c r="A1470" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C1470">
+        <v>0</v>
+      </c>
+      <c r="D1470">
+        <v>0</v>
+      </c>
+      <c r="E1470">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:5">
+      <c r="A1471" s="1" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C1471">
+        <v>19.00032971832463</v>
+      </c>
+      <c r="D1471">
+        <v>19.00032971832463</v>
+      </c>
+      <c r="E1471">
+        <v>19.00032971832463</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:5">
+      <c r="A1472" s="1" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C1472">
+        <v>19.4693353446468</v>
+      </c>
+      <c r="D1472">
+        <v>19.37580411701953</v>
+      </c>
+      <c r="E1472">
+        <v>19.24772766594151</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:5">
+      <c r="A1473" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C1473">
+        <v>16.63789607831781</v>
+      </c>
+      <c r="D1473">
+        <v>16.63789607831781</v>
+      </c>
+      <c r="E1473">
+        <v>16.63789607831781</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:5">
+      <c r="A1474" s="1" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C1474">
+        <v>19.27171326363419</v>
+      </c>
+      <c r="D1474">
+        <v>19.28558597677667</v>
+      </c>
+      <c r="E1474">
+        <v>19.28381182603322</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:5">
+      <c r="A1475" s="1" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C1475">
+        <v>10.1945169955856</v>
+      </c>
+      <c r="D1475">
+        <v>10.1945169955856</v>
+      </c>
+      <c r="E1475">
+        <v>10.1945169955856</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:5">
+      <c r="A1476" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C1476">
+        <v>11.15606071240911</v>
+      </c>
+      <c r="D1476">
+        <v>11.04595970731102</v>
+      </c>
+      <c r="E1476">
+        <v>10.92233902608439</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:5">
+      <c r="A1477" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C1477">
+        <v>4.423537535334355</v>
+      </c>
+      <c r="D1477">
+        <v>4.423537535334355</v>
+      </c>
+      <c r="E1477">
+        <v>4.423537535334355</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:5">
+      <c r="A1478" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C1478">
+        <v>4.318931062344308</v>
+      </c>
+      <c r="D1478">
+        <v>4.312667561891613</v>
+      </c>
+      <c r="E1478">
+        <v>4.313317859992234</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:5">
+      <c r="A1479" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C1479">
+        <v>25.71537651982733</v>
+      </c>
+      <c r="D1479">
+        <v>25.71537651982733</v>
+      </c>
+      <c r="E1479">
+        <v>25.71537651982733</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:5">
+      <c r="A1480" s="1" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C1480">
+        <v>28.19310963582926</v>
+      </c>
+      <c r="D1480">
+        <v>27.03759665161701</v>
+      </c>
+      <c r="E1480">
+        <v>26.71540738503945</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:5">
+      <c r="A1481" s="1" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C1481">
+        <v>9.893383537176318</v>
+      </c>
+      <c r="D1481">
+        <v>9.893383537176318</v>
+      </c>
+      <c r="E1481">
+        <v>9.893383537176318</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:5">
+      <c r="A1482" s="1" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C1482">
+        <v>9.956893577718436</v>
+      </c>
+      <c r="D1482">
+        <v>9.956915770717734</v>
+      </c>
+      <c r="E1482">
+        <v>9.956923310275558</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:5">
+      <c r="A1483" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="C1483">
+        <v>0</v>
+      </c>
+      <c r="D1483">
+        <v>0</v>
+      </c>
+      <c r="E1483">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:5">
+      <c r="A1484" s="1" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C1484">
+        <v>0</v>
+      </c>
+      <c r="D1484">
+        <v>0</v>
+      </c>
+      <c r="E1484">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:5">
+      <c r="A1485" s="1" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C1485">
+        <v>9.000384485519868</v>
+      </c>
+      <c r="D1485">
+        <v>9.000384485519868</v>
+      </c>
+      <c r="E1485">
+        <v>9.000384485519868</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:5">
+      <c r="A1486" s="1" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C1486">
+        <v>9.360846884237608</v>
+      </c>
+      <c r="D1486">
+        <v>9.382152700650103</v>
+      </c>
+      <c r="E1486">
+        <v>9.374972223665662</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:5">
+      <c r="A1487" s="1" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C1487">
+        <v>4.816265316393286</v>
+      </c>
+      <c r="D1487">
+        <v>4.816265316393286</v>
+      </c>
+      <c r="E1487">
+        <v>4.816265316393286</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:5">
+      <c r="A1488" s="1" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C1488">
+        <v>5.21737476075624</v>
+      </c>
+      <c r="D1488">
+        <v>5.207898905781394</v>
+      </c>
+      <c r="E1488">
+        <v>5.208887551814326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - add calculate_growth_percentage function
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df_fixed_1.xlsx
+++ b/create_forecast_basic/utils/monitoring_df_fixed_1.xlsx
@@ -40,19 +40,19 @@
     <t>emp_2050</t>
   </si>
   <si>
-    <t>Taz_U_Jewish</t>
-  </si>
-  <si>
-    <t>Taz_U_U_Orthodox</t>
-  </si>
-  <si>
-    <t>Taz_U_Palestinian</t>
-  </si>
-  <si>
-    <t>Taz_U_Arab</t>
-  </si>
-  <si>
-    <t>Taz_U_arabs_behined_seperation_wall</t>
+    <t>Taz_nums for Jewish sector</t>
+  </si>
+  <si>
+    <t>Taz_nums for U_Orthodox sector</t>
+  </si>
+  <si>
+    <t>Taz_nums for Palestinian sector</t>
+  </si>
+  <si>
+    <t>Taz_nums for Arab sector</t>
+  </si>
+  <si>
+    <t>Taz_nums for arabs_behined_seperation_wall sector</t>
   </si>
   <si>
     <t>univ_2020</t>

</xml_diff>